<commit_message>
naming files n shtuff/QA on PIFL47
</commit_message>
<xml_diff>
--- a/data/Experiment/Raw/Fluorescence/Fluorescence_08042025.xlsx
+++ b/data/Experiment/Raw/Fluorescence/Fluorescence_08042025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernbromley/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernbromley/Desktop/SeedlingMortality/data/Experiment/Raw/Fluorescence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FECAFE-9AEF-3E4E-AFF9-398AF3CC7A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2839CA79-60CD-C340-8E47-D70E81B78A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17060" activeTab="3" xr2:uid="{CA551DF1-0ED1-674A-8F89-05216640288A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="13080" windowHeight="17060" activeTab="2" xr2:uid="{CA551DF1-0ED1-674A-8F89-05216640288A}"/>
   </bookViews>
   <sheets>
     <sheet name="PIPO" sheetId="1" r:id="rId1"/>
@@ -690,7 +690,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView zoomScale="159" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -877,7 +877,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView zoomScale="157" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1062,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B18CAA-D5E2-8F4D-8617-88F8364D5DB9}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView zoomScale="160" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1204,7 +1204,7 @@
         <v>36</v>
       </c>
       <c r="B17" s="4">
-        <v>0.63</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1248,7 +1248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115E6809-C6E9-4B42-AF0B-D16D811C3B7F}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
+    <sheetView zoomScale="168" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>